<commit_message>
final + max + tabelka
</commit_message>
<xml_diff>
--- a/Tabela.xlsx
+++ b/Tabela.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24180" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Nazwa</t>
   </si>
@@ -30,15 +30,9 @@
     <t>Energia</t>
   </si>
   <si>
-    <t>Energia po skanowaniu</t>
-  </si>
-  <si>
     <t>Entropia</t>
   </si>
   <si>
-    <t>Entropia po skanowaniu</t>
-  </si>
-  <si>
     <t>ATrain.wav</t>
   </si>
   <si>
@@ -93,13 +87,37 @@
     <t>Średnia</t>
   </si>
   <si>
-    <t>Entropia ze współczynnikiem</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
     <t>średnia entropia</t>
+  </si>
+  <si>
+    <t>Energia po kodowaniu róznicowym</t>
+  </si>
+  <si>
+    <t>Entropia po kodowaniu różnicowym</t>
+  </si>
+  <si>
+    <t>Entropia po kodowaniu predykcyjnym MMSE r = 3</t>
+  </si>
+  <si>
+    <t>Entropia po kodowaniu predykcyjnym MMSE r = 40</t>
+  </si>
+  <si>
+    <t>kanał lewy r = 3</t>
+  </si>
+  <si>
+    <t>kanał lewy r = 10</t>
+  </si>
+  <si>
+    <t>kanał prawy r = 3</t>
+  </si>
+  <si>
+    <t>kanał prawy r = 10</t>
+  </si>
+  <si>
+    <t>Suma współczynników predykcji ATrain</t>
   </si>
 </sst>
 </file>
@@ -135,13 +153,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1481,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I63"/>
+  <dimension ref="B2:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,15 +1513,16 @@
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" customWidth="1"/>
+    <col min="9" max="9" width="45" customWidth="1"/>
+    <col min="10" max="10" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1512,24 +1534,27 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>1688526</v>
@@ -1549,13 +1574,16 @@
       <c r="I3">
         <v>8.800084</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>8.3484789999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>1378518</v>
@@ -1575,13 +1603,16 @@
       <c r="I4">
         <v>10.547815</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>10.321882</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>1063080</v>
@@ -1601,13 +1632,16 @@
       <c r="I5">
         <v>10.633188000000001</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>10.429010999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>1652746</v>
@@ -1627,13 +1661,16 @@
       <c r="I6">
         <v>10.320377000000001</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>10.249891999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>1764588</v>
@@ -1653,13 +1690,16 @@
       <c r="I7">
         <v>12.161030999999999</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>11.884411</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>1692318</v>
@@ -1679,13 +1719,16 @@
       <c r="I8">
         <v>9.2468850000000007</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>8.7656019999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>1764384</v>
@@ -1705,13 +1748,16 @@
       <c r="I9">
         <v>11.624713</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>11.595592999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>1765496</v>
@@ -1731,13 +1777,16 @@
       <c r="I10">
         <v>11.35665</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>10.951558</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>1749206</v>
@@ -1757,13 +1806,16 @@
       <c r="I11">
         <v>11.177764</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>10.908531</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>1756156</v>
@@ -1783,13 +1835,16 @@
       <c r="I12">
         <v>11.386552999999999</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>10.881966</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>1540674</v>
@@ -1809,13 +1864,16 @@
       <c r="I13">
         <v>10.227458</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>9.8779439999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>1583468</v>
@@ -1835,13 +1893,16 @@
       <c r="I14">
         <v>8.2622079999999993</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>7.7674969999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15">
         <v>1604472</v>
@@ -1861,13 +1922,16 @@
       <c r="I15">
         <v>12.514480000000001</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>12.207444000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16">
         <v>1703930</v>
@@ -1887,13 +1951,16 @@
       <c r="I16">
         <v>11.942791</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>11.728142999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>1751498</v>
@@ -1913,13 +1980,16 @@
       <c r="I17">
         <v>9.6323019999999993</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>9.2193959999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18">
         <v>1047684</v>
@@ -1939,10 +2009,13 @@
       <c r="I18">
         <v>12.013982</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>11.802412</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2">
         <f>SUM(D3:D18)/16</f>
@@ -1968,16 +2041,20 @@
         <f t="shared" si="0"/>
         <v>10.740517562499999</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="2">
+        <f>SUM(J3:J18)/16</f>
+        <v>10.4337350625</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>3</v>
       </c>
@@ -1985,47 +2062,74 @@
         <v>10.740500000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>4</v>
       </c>
       <c r="C27" s="2">
         <v>10.6203</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>5</v>
       </c>
       <c r="C28" s="2">
         <v>10.604799999999999</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28">
+        <v>0.97889999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>6</v>
       </c>
       <c r="C29" s="2">
         <v>10.572699999999999</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29">
+        <v>0.97489999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>7</v>
       </c>
       <c r="C30" s="2">
         <v>10.566000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30">
+        <v>0.95740000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>8</v>
       </c>
       <c r="C31" s="2">
         <v>10.541600000000001</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31">
+        <v>0.93220000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
lecimy do 600 xD
</commit_message>
<xml_diff>
--- a/Tabela.xlsx
+++ b/Tabela.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Nazwa</t>
   </si>
@@ -691,220 +691,114 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$B$70:$B$99</c:f>
+              <c:f>Arkusz1!$B$137:$B$150</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="12">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>290</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$C$70:$C$99</c:f>
+              <c:f>Arkusz1!$C$137:$C$150</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>9.1875</c:v>
+                  <c:v>10.680300000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.4375</c:v>
+                  <c:v>10.627599999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.375</c:v>
+                  <c:v>10.6442</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.1875</c:v>
+                  <c:v>10.8001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9375</c:v>
+                  <c:v>10.6791</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.6875</c:v>
+                  <c:v>10.803100000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.875</c:v>
+                  <c:v>10.6218</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.0625</c:v>
+                  <c:v>10.856400000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.5</c:v>
+                  <c:v>10.832800000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.4375</c:v>
+                  <c:v>10.8543</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.25</c:v>
+                  <c:v>10.8809</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.1875</c:v>
+                  <c:v>10.853400000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.375</c:v>
+                  <c:v>10.907</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.9375</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11.375</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11.1875</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>11.0625</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11.5625</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11.1875</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11.6875</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11.8125</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11.75</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>10.875</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>11.8125</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>11.875</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>11.875</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>11.6875</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>12.25</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>11.8125</c:v>
+                  <c:v>10.929500000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -912,7 +806,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-59D0-43ED-B715-506E2E579F92}"/>
+              <c16:uniqueId val="{00000000-E16F-4E2C-9EDB-6281A6F4F381}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -924,11 +818,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106414239"/>
-        <c:axId val="106429215"/>
+        <c:axId val="750742895"/>
+        <c:axId val="749812863"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106414239"/>
+        <c:axId val="750742895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,12 +879,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106429215"/>
+        <c:crossAx val="749812863"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106429215"/>
+        <c:axId val="749812863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +941,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106414239"/>
+        <c:crossAx val="750742895"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2242,20 +2136,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>29135</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>179293</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="4" name="Wykres 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2538,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3419,15 +3313,18 @@
         <v>10.7569</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="5">
         <v>10</v>
       </c>
@@ -3435,7 +3332,7 @@
         <v>9.1875</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="5">
         <v>20</v>
       </c>
@@ -3443,7 +3340,7 @@
         <v>9.4375</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="5">
         <v>30</v>
       </c>
@@ -3451,7 +3348,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="5">
         <v>40</v>
       </c>
@@ -3459,7 +3356,7 @@
         <v>9.1875</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="5">
         <v>50</v>
       </c>
@@ -3467,7 +3364,7 @@
         <v>9.9375</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="5">
         <v>60</v>
       </c>
@@ -3475,7 +3372,7 @@
         <v>9.6875</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="5">
         <v>70</v>
       </c>
@@ -3483,7 +3380,7 @@
         <v>10.875</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="5">
         <v>80</v>
       </c>
@@ -3491,7 +3388,7 @@
         <v>10.0625</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="5">
         <v>90</v>
       </c>
@@ -3499,7 +3396,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="5">
         <v>100</v>
       </c>
@@ -3507,7 +3404,7 @@
         <v>10.4375</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="5">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
odpal to dla beki xD
</commit_message>
<xml_diff>
--- a/Tabela.xlsx
+++ b/Tabela.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Nazwa</t>
   </si>
@@ -129,7 +129,10 @@
     <t>minLsr</t>
   </si>
   <si>
-    <t>&lt;= minimum</t>
+    <t>minLsr z podziałem</t>
+  </si>
+  <si>
+    <t>minimum</t>
   </si>
 </sst>
 </file>
@@ -156,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -164,11 +167,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,6 +220,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -212,7 +263,68 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Średnia</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> entropia dla wszystkich plików po kodowaniu predykcyjnym MMSE</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -680,7 +792,68 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>b &lt; 5; 24</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> &gt;</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -691,114 +864,400 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$B$137:$B$150</c:f>
+              <c:f>Arkusz1!$B$70:$B$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>120</c:v>
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$C$137:$C$150</c:f>
+              <c:f>Arkusz1!$C$70:$C$129</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="60"/>
                 <c:pt idx="0">
-                  <c:v>10.680300000000001</c:v>
+                  <c:v>9.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.627599999999999</c:v>
+                  <c:v>9.5625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.6442</c:v>
+                  <c:v>8.9375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.8001</c:v>
+                  <c:v>10.0625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.6791</c:v>
+                  <c:v>10.375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.803100000000001</c:v>
+                  <c:v>10.4375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.6218</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.856400000000001</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.832800000000001</c:v>
+                  <c:v>11.125</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.8543</c:v>
+                  <c:v>11.125</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.8809</c:v>
+                  <c:v>11.3125</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.853400000000001</c:v>
+                  <c:v>11.875</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.907</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.929500000000001</c:v>
+                  <c:v>12.125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.4375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.4375</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11.6875</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.1875</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12.1875</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.4375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.1875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.375</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12.3125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.0625</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.375</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12.0625</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.5625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11.9375</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.375</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12.4375</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.125</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12.4375</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.625</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.75</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.5625</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12.1875</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12.8125</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12.8125</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12.3125</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>12.5625</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12.375</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12.5625</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.875</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>12.8125</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12.75</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>12.8125</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>12.75</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>12.625</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>12.625</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>12.5625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,7 +1265,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E16F-4E2C-9EDB-6281A6F4F381}"/>
+              <c16:uniqueId val="{00000000-C65B-480B-9349-9395CEB74EAB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -818,11 +1277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="750742895"/>
-        <c:axId val="749812863"/>
+        <c:axId val="761080992"/>
+        <c:axId val="761071840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="750742895"/>
+        <c:axId val="761080992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -879,12 +1338,12 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749812863"/>
+        <c:crossAx val="761071840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="749812863"/>
+        <c:axId val="761071840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +1400,668 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="750742895"/>
+        <c:crossAx val="761080992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>minLsr &lt; 5; 24</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> &gt;</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz1!$B$70:$B$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz1!$D$70:$D$129</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>11.252800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.289300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.3705</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.502700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.5708</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.613899999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.738799999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.797499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.8233</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.7942</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.8276</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.834</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.8576</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.9513</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.058199999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.033099999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.063000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12.001200000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.078099999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12.0738</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12.077299999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.0924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12.079499999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12.1343</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.1449</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.176399999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12.188499999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.207100000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.1791</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.2835</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12.2011</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>12.214499999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12.2576</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.256</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12.2684</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.218400000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12.2667</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.2286</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>12.305999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>12.324999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12.3657</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.3368</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12.3781</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12.4305</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12.3377</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>12.328900000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12.383100000000001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>12.4437</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>12.379300000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>12.4063</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.4442</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12.4511</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>12.4572</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12.429</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>12.487399999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>12.442399999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>12.48</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>12.4519</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>12.4596</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>12.4899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCE4-4C7D-BC98-6286B51D6C6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="761066432"/>
+        <c:axId val="761066848"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="761066432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761066848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="761066848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761066432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1070,6 +2190,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1587,6 +2747,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2137,19 +3813,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>136</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1819275</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Wykres 3"/>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2159,6 +3835,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1800225</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2432,8 +4138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,412 +5034,661 @@
       <c r="B70" s="5">
         <v>10</v>
       </c>
-      <c r="C70">
-        <v>9.1875</v>
+      <c r="C70" s="2">
+        <v>9.25</v>
+      </c>
+      <c r="D70" s="2">
+        <v>11.252800000000001</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="5">
         <v>20</v>
       </c>
-      <c r="C71">
-        <v>9.4375</v>
+      <c r="C71" s="2">
+        <v>9.5625</v>
+      </c>
+      <c r="D71" s="2">
+        <v>11.289300000000001</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="5">
         <v>30</v>
       </c>
-      <c r="C72">
-        <v>9.375</v>
+      <c r="C72" s="2">
+        <v>8.9375</v>
+      </c>
+      <c r="D72" s="2">
+        <v>11.3705</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="5">
         <v>40</v>
       </c>
-      <c r="C73">
-        <v>9.1875</v>
+      <c r="C73" s="2">
+        <v>10.0625</v>
+      </c>
+      <c r="D73" s="2">
+        <v>11.502700000000001</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="5">
         <v>50</v>
       </c>
-      <c r="C74">
-        <v>9.9375</v>
+      <c r="C74" s="2">
+        <v>10.375</v>
+      </c>
+      <c r="D74" s="2">
+        <v>11.5708</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="5">
         <v>60</v>
       </c>
-      <c r="C75">
-        <v>9.6875</v>
+      <c r="C75" s="2">
+        <v>10.4375</v>
+      </c>
+      <c r="D75" s="2">
+        <v>11.613899999999999</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="5">
         <v>70</v>
       </c>
-      <c r="C76">
-        <v>10.875</v>
+      <c r="C76" s="2">
+        <v>11</v>
+      </c>
+      <c r="D76" s="2">
+        <v>11.738799999999999</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="5">
         <v>80</v>
       </c>
-      <c r="C77">
-        <v>10.0625</v>
+      <c r="C77" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="D77" s="2">
+        <v>11.797499999999999</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="5">
         <v>90</v>
       </c>
-      <c r="C78">
-        <v>10.5</v>
+      <c r="C78" s="2">
+        <v>11.125</v>
+      </c>
+      <c r="D78" s="2">
+        <v>11.8233</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="5">
         <v>100</v>
       </c>
-      <c r="C79">
-        <v>10.4375</v>
+      <c r="C79" s="2">
+        <v>11.125</v>
+      </c>
+      <c r="D79" s="2">
+        <v>11.7942</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="5">
         <v>110</v>
       </c>
-      <c r="C80">
-        <v>11.25</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="2">
+        <v>11.3125</v>
+      </c>
+      <c r="D80" s="2">
+        <v>11.8276</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="5">
         <v>120</v>
       </c>
-      <c r="C81">
-        <v>11.1875</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="2">
+        <v>11.875</v>
+      </c>
+      <c r="D81" s="2">
+        <v>11.834</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="5">
         <v>130</v>
       </c>
-      <c r="C82">
-        <v>11.375</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="D82" s="2">
+        <v>11.8576</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="5">
         <v>140</v>
       </c>
-      <c r="C83">
-        <v>11.9375</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="2">
+        <v>12.125</v>
+      </c>
+      <c r="D83" s="2">
+        <v>11.9513</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="5">
         <v>150</v>
       </c>
-      <c r="C84">
-        <v>11.375</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="2">
+        <v>12</v>
+      </c>
+      <c r="D84" s="2">
+        <v>12.058199999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="5">
         <v>160</v>
       </c>
-      <c r="C85">
-        <v>11.1875</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="2">
+        <v>11.4375</v>
+      </c>
+      <c r="D85" s="2">
+        <v>12.033099999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="5">
         <v>170</v>
       </c>
-      <c r="C86">
-        <v>11.0625</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="2">
+        <v>11.4375</v>
+      </c>
+      <c r="D86" s="2">
+        <v>12.063000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="5">
         <v>180</v>
       </c>
-      <c r="C87">
-        <v>11.5625</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="2">
+        <v>12</v>
+      </c>
+      <c r="D87" s="2">
+        <v>12.001200000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="5">
         <v>190</v>
       </c>
-      <c r="C88">
-        <v>11.1875</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="2">
+        <v>11.6875</v>
+      </c>
+      <c r="D88" s="2">
+        <v>12.078099999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="5">
         <v>200</v>
       </c>
-      <c r="C89">
-        <v>11.6875</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="2">
+        <v>12.1875</v>
+      </c>
+      <c r="D89" s="2">
+        <v>12.0738</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="5">
         <v>210</v>
       </c>
-      <c r="C90">
-        <v>11.8125</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="2">
+        <v>12.1875</v>
+      </c>
+      <c r="D90" s="2">
+        <v>12.077299999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="5">
         <v>220</v>
       </c>
-      <c r="C91">
-        <v>11.75</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="2">
+        <v>12</v>
+      </c>
+      <c r="D91" s="2">
+        <v>12.0924</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="5">
         <v>230</v>
       </c>
-      <c r="C92">
-        <v>10.875</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="2">
+        <v>11.4375</v>
+      </c>
+      <c r="D92" s="2">
+        <v>12.079499999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="5">
         <v>240</v>
       </c>
-      <c r="C93">
-        <v>11.8125</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="2">
+        <v>12.1875</v>
+      </c>
+      <c r="D93" s="2">
+        <v>12.1343</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="5">
         <v>250</v>
       </c>
-      <c r="C94">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="2">
+        <v>12.25</v>
+      </c>
+      <c r="D94" s="2">
+        <v>12.1449</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="5">
         <v>260</v>
       </c>
-      <c r="C95">
-        <v>11.875</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="2">
+        <v>12.375</v>
+      </c>
+      <c r="D95" s="2">
+        <v>12.176399999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="5">
         <v>270</v>
       </c>
-      <c r="C96">
-        <v>11.875</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="2">
+        <v>12.3125</v>
+      </c>
+      <c r="D96" s="2">
+        <v>12.188499999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="5">
         <v>280</v>
       </c>
-      <c r="C97">
-        <v>11.6875</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="2">
+        <v>12.0625</v>
+      </c>
+      <c r="D97" s="2">
+        <v>12.207100000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="5">
         <v>290</v>
       </c>
-      <c r="C98">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="2">
+        <v>12.375</v>
+      </c>
+      <c r="D98" s="2">
+        <v>12.1791</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="5">
         <v>300</v>
       </c>
-      <c r="C99">
-        <v>11.8125</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="2">
+        <v>12.125</v>
+      </c>
+      <c r="D99" s="2">
+        <v>12.2835</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="5">
         <v>310</v>
       </c>
-      <c r="C100">
-        <v>11.875</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="2">
+        <v>12.0625</v>
+      </c>
+      <c r="D100" s="2">
+        <v>12.2011</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="5">
         <v>320</v>
       </c>
-      <c r="C101">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="2">
+        <v>12.5625</v>
+      </c>
+      <c r="D101" s="2">
+        <v>12.214499999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="5">
         <v>330</v>
       </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="2">
+        <v>11.9375</v>
+      </c>
+      <c r="D102" s="2">
+        <v>12.2576</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="5">
         <v>340</v>
       </c>
-      <c r="C103">
-        <v>11.9375</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="2">
+        <v>12.375</v>
+      </c>
+      <c r="D103" s="2">
+        <v>12.256</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="5">
         <v>350</v>
       </c>
-      <c r="C104">
-        <v>11.75</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="2">
+        <v>12.4375</v>
+      </c>
+      <c r="D104" s="2">
+        <v>12.2684</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="5">
         <v>360</v>
       </c>
-      <c r="C105">
-        <v>11.9375</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="2">
+        <v>12.125</v>
+      </c>
+      <c r="D105" s="2">
+        <v>12.218400000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="5">
         <v>370</v>
       </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="2">
+        <v>12.4375</v>
+      </c>
+      <c r="D106" s="2">
+        <v>12.2667</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B107" s="5">
         <v>380</v>
       </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="2">
+        <v>12.25</v>
+      </c>
+      <c r="D107" s="2">
+        <v>12.2286</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="5">
         <v>390</v>
       </c>
-      <c r="C108">
-        <v>12.375</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="2">
+        <v>12.625</v>
+      </c>
+      <c r="D108" s="2">
+        <v>12.305999999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="5">
         <v>400</v>
       </c>
-      <c r="C109">
-        <v>12.25</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="2">
+        <v>12.375</v>
+      </c>
+      <c r="D109" s="2">
+        <v>12.324999999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="5">
         <v>410</v>
       </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="2">
+        <v>12.75</v>
+      </c>
+      <c r="D110" s="2">
+        <v>12.3657</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="5">
         <v>420</v>
       </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="2">
+        <v>12.5625</v>
+      </c>
+      <c r="D111" s="2">
+        <v>12.3368</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="5">
         <v>430</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C112" s="2">
+        <v>12.1875</v>
+      </c>
+      <c r="D112" s="2">
+        <v>12.3781</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="5">
         <v>440</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C113" s="2">
+        <v>12.8125</v>
+      </c>
+      <c r="D113" s="2">
+        <v>12.4305</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="5">
         <v>450</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C114" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="D114" s="2">
+        <v>12.3377</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="5">
         <v>460</v>
       </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C115" s="2">
+        <v>12.8125</v>
+      </c>
+      <c r="D115" s="2">
+        <v>12.328900000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="5">
         <v>470</v>
       </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C116" s="2">
+        <v>12.3125</v>
+      </c>
+      <c r="D116" s="2">
+        <v>12.383100000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="5">
         <v>480</v>
       </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C117" s="2">
+        <v>12.5625</v>
+      </c>
+      <c r="D117" s="2">
+        <v>12.4437</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="5">
         <v>490</v>
       </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C118" s="2">
+        <v>12.375</v>
+      </c>
+      <c r="D118" s="2">
+        <v>12.379300000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="5">
         <v>500</v>
       </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C119" s="2">
+        <v>12.5625</v>
+      </c>
+      <c r="D119" s="2">
+        <v>12.4063</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="5">
         <v>510</v>
       </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C120" s="2">
+        <v>12.875</v>
+      </c>
+      <c r="D120" s="2">
+        <v>12.4442</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="5">
         <v>520</v>
       </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C121" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="D121" s="2">
+        <v>12.4511</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="5">
         <v>530</v>
       </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C122" s="2">
+        <v>12.8125</v>
+      </c>
+      <c r="D122" s="2">
+        <v>12.4572</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="5">
         <v>540</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C123" s="2">
+        <v>12.25</v>
+      </c>
+      <c r="D123" s="2">
+        <v>12.429</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="5">
         <v>550</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C124" s="2">
+        <v>12.75</v>
+      </c>
+      <c r="D124" s="2">
+        <v>12.487399999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="5">
         <v>560</v>
       </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C125" s="2">
+        <v>12.8125</v>
+      </c>
+      <c r="D125" s="2">
+        <v>12.442399999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="5">
         <v>570</v>
       </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C126" s="2">
+        <v>12.75</v>
+      </c>
+      <c r="D126" s="2">
+        <v>12.48</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="5">
         <v>580</v>
       </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C127" s="2">
+        <v>12.625</v>
+      </c>
+      <c r="D127" s="2">
+        <v>12.4519</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="5">
         <v>590</v>
+      </c>
+      <c r="C128" s="2">
+        <v>12.625</v>
+      </c>
+      <c r="D128" s="2">
+        <v>12.4596</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="5">
         <v>600</v>
       </c>
+      <c r="C129" s="2">
+        <v>12.5625</v>
+      </c>
+      <c r="D129" s="2">
+        <v>12.4899</v>
+      </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
@@ -3743,7 +5698,7 @@
         <v>22</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,30 +5762,30 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="1">
+      <c r="A142" s="8">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B142" s="1">
+      <c r="B142" s="8">
         <v>10</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="6">
         <v>10.803100000000001</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+      <c r="A143" s="10">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="9">
         <v>12</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="7">
         <v>10.6218</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>